<commit_message>
Added automatic step-by-step generation
</commit_message>
<xml_diff>
--- a/Documents/DTT-Assessment-Hour-Log.xlsx
+++ b/Documents/DTT-Assessment-Hour-Log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[Projects]\Unity\DTT Assessment - Unity\DTT Assessment - Unity - 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[Projects]\Unity\A Mazing\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18320407-56ED-44D1-9C16-E2A31EC5FEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CB302C-61D6-465E-B5FE-FF959B8B2BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>Subject</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Wrote a small document explaining some of the choices I made and a description of my classes.</t>
+  </si>
+  <si>
+    <t>Made automatic step by step generator</t>
+  </si>
+  <si>
+    <t>Made a system  + UI to let the maze generate in steps automatically, so you can see the algorithm at work.</t>
   </si>
 </sst>
 </file>
@@ -1819,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2130,12 +2136,22 @@
       <c r="E18" s="19"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="19"/>
+    <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="18">
+        <v>45273</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>